<commit_message>
add column and remove columns
</commit_message>
<xml_diff>
--- a/DA_panda/vehicle_data.xlsx
+++ b/DA_panda/vehicle_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="44">
   <si>
     <t>name</t>
   </si>
@@ -31,6 +31,9 @@
     <t>vehicle</t>
   </si>
   <si>
+    <t>country</t>
+  </si>
+  <si>
     <t>harihar</t>
   </si>
   <si>
@@ -94,27 +97,30 @@
     <t>bangalore</t>
   </si>
   <si>
+    <t>surat</t>
+  </si>
+  <si>
+    <t>jaipur</t>
+  </si>
+  <si>
+    <t>pune</t>
+  </si>
+  <si>
+    <t>mumbai</t>
+  </si>
+  <si>
+    <t>haridwar</t>
+  </si>
+  <si>
+    <t>hyderabad</t>
+  </si>
+  <si>
+    <t>bhubaneswar</t>
+  </si>
+  <si>
     <t>noida</t>
   </si>
   <si>
-    <t>surat</t>
-  </si>
-  <si>
-    <t>jaipur</t>
-  </si>
-  <si>
-    <t>pune</t>
-  </si>
-  <si>
-    <t>mumbai</t>
-  </si>
-  <si>
-    <t>haridwar</t>
-  </si>
-  <si>
-    <t>hyderabad</t>
-  </si>
-  <si>
     <t>BMW</t>
   </si>
   <si>
@@ -137,6 +143,9 @@
   </si>
   <si>
     <t>Mercedes</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -494,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,47 +525,56 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>28</v>
@@ -565,15 +583,18 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>23</v>
@@ -582,15 +603,18 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>55</v>
@@ -599,15 +623,18 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>43</v>
@@ -616,15 +643,18 @@
         <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>48</v>
@@ -633,15 +663,18 @@
         <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>33</v>
@@ -650,15 +683,18 @@
         <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -667,66 +703,78 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>23</v>
@@ -735,32 +783,38 @@
         <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>43</v>
@@ -769,15 +823,18 @@
         <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>44</v>
@@ -786,15 +843,18 @@
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>33</v>
@@ -803,15 +863,18 @@
         <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19">
         <v>25</v>
@@ -820,7 +883,10 @@
         <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>